<commit_message>
return, variance and performance calculations work
</commit_message>
<xml_diff>
--- a/PyCharm Projects/3. assignment_2/Diversification-Tool-3.xlsx
+++ b/PyCharm Projects/3. assignment_2/Diversification-Tool-3.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t xml:space="preserve">To calculate your current performance please enter numbers in colored cells.</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t xml:space="preserve">Stock C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StockC</t>
   </si>
   <si>
     <t xml:space="preserve">Penalty for risk  b=</t>
@@ -517,8 +514,8 @@
   </sheetPr>
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N8" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U28" activeCellId="0" sqref="U28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H6" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -796,11 +793,11 @@
         <v>750</v>
       </c>
       <c r="Z8" s="13" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="AA8" s="5" t="n">
         <f aca="false">1/4*(W8+X8+Y8+Z8)</f>
-        <v>275</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,8 +823,7 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="16" t="n">
-        <f aca="false">B9+D9-E9</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>19</v>
@@ -892,8 +888,7 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="16" t="n">
-        <f aca="false">B10+D10-E10</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>21</v>
@@ -958,11 +953,10 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="16" t="n">
-        <f aca="false">B11+D11-E11</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -995,8 +989,7 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="16" t="n">
-        <f aca="false">B12+D12-E12</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>22</v>
@@ -1019,7 +1012,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="22" t="n">
@@ -1057,11 +1050,11 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P14" s="5" t="n">
         <f aca="false">J8+J9*1/4*(Q7+R7+S7+T7)+J10*1/4*(Q8+R8+S8+T8)+J12*1/4*(Q10+R10+S10+T10) + J11*1/4*(Q9+R9+S9+T9)</f>
-        <v>108.47</v>
+        <v>403.47</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="V14" s="8"/>
@@ -1085,7 +1078,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="V15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W15" s="8" t="n">
         <f aca="false">W7^2</f>
@@ -1119,7 +1112,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="V16" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W16" s="8" t="n">
         <f aca="false">W8^2</f>
@@ -1135,7 +1128,7 @@
       </c>
       <c r="Z16" s="13" t="n">
         <f aca="false">Z8^2</f>
-        <v>10000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1153,7 +1146,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="V17" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W17" s="8" t="n">
         <f aca="false">W9^2</f>
@@ -1187,14 +1180,14 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="T18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U18" s="5" t="n">
         <f aca="false">1/4*(W15+X15+Y15+Z15)-1/16*(W7+X7+Y7+Z7)^2</f>
         <v>156250</v>
       </c>
       <c r="V18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W18" s="8" t="n">
         <f aca="false">W10^2</f>
@@ -1227,11 +1220,11 @@
       <c r="K19" s="2"/>
       <c r="M19" s="2"/>
       <c r="T19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U19" s="5" t="n">
         <f aca="false">1/4*(W16+X16+Y16+Z16)-1/16*(W8+X8+Y8+Z8)^2</f>
-        <v>83125</v>
+        <v>156250</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,16 +1238,16 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K20" s="27"/>
       <c r="L20" s="28" t="n">
         <f aca="false">P14-P13*P25</f>
-        <v>-33172.78</v>
+        <v>-1124596.53</v>
       </c>
       <c r="M20" s="29"/>
       <c r="T20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U20" s="5" t="n">
         <f aca="false">1/4*(W17+X17+Y17+Z17)-1/16*(W9+X9+Y9+Z9)^2</f>
@@ -1272,18 +1265,18 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K21" s="29"/>
       <c r="L21" s="29" t="n">
         <f aca="false">P14/SQRT(P25)</f>
-        <v>0.0594579354839939</v>
+        <v>0.0380395164007115</v>
       </c>
       <c r="M21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T21" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="U21" s="5" t="n">
         <f aca="false">1/4*(W18+X18+Y18+Z18)-1/16*(W10+X10+Y10+Z10)^2</f>
@@ -1301,16 +1294,16 @@
     </row>
     <row r="23" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U23" s="5" t="n">
         <f aca="false">1/4*(W7*W8+X7*X8+Y7*Y8+Z7*Z8)-AA7*AA8</f>
-        <v>9375</v>
+        <v>-46875</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U24" s="5" t="n">
         <f aca="false">1/4*(W7*W10+X7*X10+Y7*Y10+Z7*Z10)-AA7*AA10</f>
@@ -1319,14 +1312,14 @@
     </row>
     <row r="25" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P25" s="5" t="n">
         <f aca="false">J9^2*U18+J10^2*U19+J11^2*U20+J12^2*U21+2*J9*J10*U23+2*J9*J12*U24+2*J10*J12*U25 + 2*J11*J12*U26+2*J9*J11*U27+2*J10*J11*U28</f>
-        <v>3328125</v>
+        <v>112500000</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U25" s="5" t="n">
         <f aca="false">1/4*(W8*W10+X8*X10+Y8*Y10+Z8*Z10)-AA8*AA10</f>
@@ -1337,7 +1330,7 @@
       <c r="G26" s="31"/>
       <c r="Q26" s="5"/>
       <c r="T26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U26" s="5" t="n">
         <f aca="false">1/4*(W9*W10+X9*X10+Y9*Y10+Z9*Z10)-AA9*AA10</f>
@@ -1346,7 +1339,7 @@
     </row>
     <row r="27" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U27" s="1" t="n">
         <f aca="false">1/4*(W7*W9+X7*X9+Y7*Y9+Z7*Z9)-AA7*AA9</f>
@@ -1355,11 +1348,11 @@
     </row>
     <row r="28" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U28" s="1" t="n">
         <f aca="false">1/4*(W8*W9+X8*X9+Y8*Y9+Z8*Z9)-AA8*AA9</f>
-        <v>-18750</v>
+        <v>93750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>